<commit_message>
Se agregaron los metodos para el llenado de las tablas de empleados y productos con la informacion alamcenada en la base de datos
</commit_message>
<xml_diff>
--- a/BaseDeDatos.xlsx
+++ b/BaseDeDatos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>Nombre</t>
   </si>
@@ -38,6 +38,9 @@
     <t>Direccion</t>
   </si>
   <si>
+    <t>Codigo</t>
+  </si>
+  <si>
     <t>Marca</t>
   </si>
   <si>
@@ -81,6 +84,123 @@
   </si>
   <si>
     <t>Domingo</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>Queso</t>
+  </si>
+  <si>
+    <t>Palmar</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>SAlchicha</t>
+  </si>
+  <si>
+    <t>oscar</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>palta</t>
+  </si>
+  <si>
+    <t>rio</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>harina</t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>pasta</t>
+  </si>
+  <si>
+    <t>fiore</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>perrarina</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>purina</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>salsa</t>
+  </si>
+  <si>
+    <t>mavesa</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Torres</t>
+  </si>
+  <si>
+    <t>luis@</t>
+  </si>
+  <si>
+    <t>luis</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>14789</t>
+  </si>
+  <si>
+    <t>Moron</t>
   </si>
 </sst>
 </file>
@@ -125,7 +245,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -154,6 +274,29 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -161,7 +304,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -169,16 +312,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -196,22 +461,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -229,31 +494,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
         <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>